<commit_message>
REMOVED image in tours
</commit_message>
<xml_diff>
--- a/public/uploads/Untitled 1.xlsx
+++ b/public/uploads/Untitled 1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,42 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t xml:space="preserve">Name</t>
+    <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">Prize</t>
+    <t xml:space="preserve">prize</t>
   </si>
   <si>
-    <t xml:space="preserve"> Joseph Talamayan </t>
+    <t xml:space="preserve">Areeya</t>
   </si>
   <si>
-    <t xml:space="preserve">John Tech </t>
+    <t xml:space="preserve">Bryan Boon Areglado</t>
   </si>
   <si>
-    <t xml:space="preserve">Florencio Campomanes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vamerdino Magsakay</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jhun Mondalo </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hazel Timonera </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Rodrigo Sequite </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Alexis Lim </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thijs Hilberts </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ruben Clamares </t>
+    <t xml:space="preserve">Adriannn</t>
   </si>
 </sst>
 </file>
@@ -65,12 +44,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -86,11 +64,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,16 +108,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -165,100 +130,44 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="210" zoomScaleNormal="210" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>50000</v>
+      <c r="B2" s="0" t="n">
+        <v>100000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>50000</v>
+      <c r="B3" s="0" t="n">
+        <v>2000000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2" t="n">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>100000</v>
+      <c r="B4" s="0" t="n">
+        <v>50000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>